<commit_message>
Doing work in manufacturer layout.  I hate gui layouts.
</commit_message>
<xml_diff>
--- a/Airplane_Master_List.xlsx
+++ b/Airplane_Master_List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t xml:space="preserve">Boeing </t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>Airbus' new wide-body twin-jet.  This uses carbon-fiber based polymers similar to the 787 for reduced weight and better fuel economy.  Replace your A330s?</t>
+  </si>
+  <si>
+    <t>Graphic File</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>boeing_787-8_cropped</t>
+  </si>
+  <si>
+    <t>B737_100</t>
   </si>
 </sst>
 </file>
@@ -419,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +447,7 @@
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -467,10 +479,13 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -502,10 +517,13 @@
         <v>224</v>
       </c>
       <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -537,10 +555,13 @@
         <v>264</v>
       </c>
       <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -572,10 +593,13 @@
         <v>306</v>
       </c>
       <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -607,10 +631,13 @@
         <v>32</v>
       </c>
       <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -642,10 +669,13 @@
         <v>40</v>
       </c>
       <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -678,6 +708,9 @@
         <v>272</v>
       </c>
       <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More graphics.  Manufacturer layout is mostly finished.  Need to work on buy button logic.
</commit_message>
<xml_diff>
--- a/Airplane_Master_List.xlsx
+++ b/Airplane_Master_List.xlsx
@@ -104,13 +104,13 @@
     <t>Graphic File</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>boeing_787-8_cropped</t>
   </si>
   <si>
     <t>B737_100</t>
+  </si>
+  <si>
+    <t>a350_900_cropped</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
         <v>224</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
         <v>17</v>
@@ -631,7 +631,7 @@
         <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
         <v>20</v>
@@ -669,7 +669,7 @@
         <v>40</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L6" t="s">
         <v>20</v>
@@ -708,7 +708,7 @@
         <v>272</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7" t="s">
         <v>24</v>

</xml_diff>